<commit_message>
[add] taff dla journee
</commit_message>
<xml_diff>
--- a/result/kopkpopok- FR0014009DK8result.xlsx
+++ b/result/kopkpopok- FR0014009DK8result.xlsx
@@ -541,7 +541,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>morgan</t>
+          <t>BNP</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>trimestre</t>
+          <t>jours</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>EURO STOXX 50 Price EUR</t>
+          <t>Bouygues SA</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>mono indice</t>
+          <t>mono action</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>50</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>31/07/2023, 30/10/2023, 29/01/2024, 29/04/2024, 29/07/2024, 29/10/2024, 29/01/2025, 29/04/2025, 29/07/2025, 29/10/2025, 29/01/2026, 29/04/2026, 29/07/2026, 29/10/2026, 29/01/2027, 29/04/2027, 29/07/2027, 29/10/2027, 31/01/2028, 02/05/2028, 31/07/2028, 30/10/2028, 29/01/2029, 30/04/2029, 30/07/2029, 29/10/2029, 29/01/2030, 29/04/2030, 29/07/2030, 29/10/2030, 29/01/2031, 29/04/2031, 29/07/2031, 29/10/2031, 29/01/2032, 29/04/2032, 29/07/2032, 29/07/2032</t>
+          <t>Chaque jour ouvré entre le 29 juillet 2023 (inclus) et le 29 juillet 2032.</t>
         </is>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>07/08/2023, 06/11/2023, 05/02/2024, 07/05/2024, 05/08/2024, 05/11/2024, 05/02/2025, 07/05/2025, 05/08/2025, 05/11/2025, 05/02/2026, 07/05/2026, 05/08/2026, 05/11/2026, 05/02/2027, 06/05/2027, 05/08/2027, 05/11/2027, 07/02/2028, 09/05/2028, 07/08/2028, 06/11/2028, 05/02/2029, 08/05/2029, 06/08/2029, 05/11/2029, 05/02/2030, 07/05/2030, 05/08/2030, 05/11/2030, 05/02/2031, 07/05/2031, 05/08/2031, 05/11/2031, 05/02/2032, 06/05/2032</t>
+          <t>Le 5e jour ouvré suivant la date de constatation quotidienne.</t>
         </is>
       </c>
     </row>

</xml_diff>